<commit_message>
Failing to reject the null hypothesis
</commit_message>
<xml_diff>
--- a/is_spending_over_100.xlsx
+++ b/is_spending_over_100.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/class_work/ttp_O31_warmups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02B361FC-5985-8248-8D29-A7C943669D06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99697F53-3F53-2A4F-BBB7-CCEF957C54F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18280" windowHeight="16440" xr2:uid="{9A028C97-ED3D-3148-978D-AD4CEEC0B584}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9A028C97-ED3D-3148-978D-AD4CEEC0B584}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>-- 2) Your boss is absolutely certain (like 99%) that his new marketing strategy will increase</t>
   </si>
@@ -109,6 +110,9 @@
   </si>
   <si>
     <t>P-value &gt; Alpha?</t>
+  </si>
+  <si>
+    <t>Conclusion: We fail to reject the null hypothesis</t>
   </si>
 </sst>
 </file>
@@ -134,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +148,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,13 +170,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDD5124-A6D0-5A4D-8A5A-43859BB2D5A3}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="132" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -575,8 +586,8 @@
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>16</v>
+      <c r="B18" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -584,7 +595,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -600,7 +611,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="2">
-        <v>102.38</v>
+        <v>102.36</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -631,7 +642,7 @@
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="4">
         <f>B23/SQRT(B21)</f>
         <v>1.0309188839617054</v>
       </c>
@@ -641,8 +652,8 @@
         <v>23</v>
       </c>
       <c r="B29" s="3">
-        <f>_xlfn.NORM.INV((1-B24), B22, B27)</f>
-        <v>104.77827595401287</v>
+        <f>_xlfn.NORM.INV((1-B24), B25, B27)</f>
+        <v>102.39827595401287</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,7 +662,7 @@
       </c>
       <c r="B30" s="4">
         <f>1 - _xlfn.NORM.DIST(B22, B25, B27,TRUE)</f>
-        <v>1.0482337323067137E-2</v>
+        <v>1.1033290152983155E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -661,6 +672,11 @@
       <c r="B31" s="3" t="b">
         <f>B30&gt;B24</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>